<commit_message>
Update Finish QR Code
</commit_message>
<xml_diff>
--- a/ShopOnline/Reports/DANH_SACH_QR_CODE.xlsx
+++ b/ShopOnline/Reports/DANH_SACH_QR_CODE.xlsx
@@ -143,7 +143,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -157,6 +157,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -166,14 +169,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -197,15 +200,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>483577</xdr:colOff>
+      <xdr:colOff>256440</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>1172</xdr:rowOff>
+      <xdr:rowOff>67115</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>679987</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>202907</xdr:rowOff>
+      <xdr:colOff>452850</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>41715</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -227,7 +230,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="483577" y="228307"/>
+          <a:off x="256440" y="294250"/>
           <a:ext cx="899795" cy="428869"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -537,18 +540,18 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="3" customWidth="1"/>
     <col min="5" max="6" width="13.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="18" style="1" customWidth="1"/>
-    <col min="8" max="8" width="23.140625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="12" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.140625" style="5" customWidth="1"/>
     <col min="9" max="9" width="9.7109375" style="1" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" style="1" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" style="1"/>
@@ -557,46 +560,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="5" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="7"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="8" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" spans="1:11" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>

</xml_diff>

<commit_message>
Update 20180815 Excel Export
</commit_message>
<xml_diff>
--- a/ShopOnline/Reports/DANH_SACH_QR_CODE.xlsx
+++ b/ShopOnline/Reports/DANH_SACH_QR_CODE.xlsx
@@ -12,7 +12,6 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">QR_Code_Export!#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">QR_Code_Export!$A$1:$J$264</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">QR_Code_Export!#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
@@ -540,7 +539,7 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -625,7 +624,7 @@
     <mergeCell ref="C3:J3"/>
     <mergeCell ref="C2:J2"/>
   </mergeCells>
-  <pageMargins left="0.98425196850393704" right="0.59055118110236227" top="0.59055118110236227" bottom="0.59055118110236227" header="0" footer="0"/>
+  <pageMargins left="0.13" right="0.13" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;10Trang &amp;P/&amp;N</oddFooter>

</xml_diff>